<commit_message>
precomputation engine+northstar API validation
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DataLoader/GenericUploader/ADTJira/Excel/Action.xlsx
+++ b/src/test/resources/testdata/DataLoader/GenericUploader/ADTJira/Excel/Action.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="883" uniqueCount="684">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="886" uniqueCount="685">
   <si>
     <t>Title</t>
   </si>
@@ -2117,6 +2117,9 @@
   </si>
   <si>
     <t>2021-05-21T07:48:06Z</t>
+  </si>
+  <si>
+    <t>2021-05-27T13:04:45Z</t>
   </si>
 </sst>
 </file>
@@ -7549,7 +7552,7 @@
       <c r="J2" s="16"/>
       <c r="K2" s="11"/>
       <c r="L2" s="11" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="M2" s="11"/>
       <c r="N2" s="11"/>

</xml_diff>

<commit_message>
GU(template chnge)+minor code change in RMP,team arch+added regressionfolder
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/DataLoader/GenericUploader/ADTJira/Excel/Action.xlsx
+++ b/src/test/resources/testdata/DataLoader/GenericUploader/ADTJira/Excel/Action.xlsx
@@ -3,14 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonal.harish.nagda\ART\ART_TestAutomationCode\src\test\resources\testdata\DataLoader\GenericUploader\ADTJira\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\l.gurulingaiah\Automation_GIT\master\src\test\resources\testdata\DataLoader\GenericUploader\ADTJira\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6875EEB-C857-43B4-981C-E380F4C00387}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D55B8BE-6C1C-441A-8FF2-ED0BB3D3110C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="680" activeTab="2" xr2:uid="{4ADEDBBA-C616-478B-B7B7-DF7FEDCE3438}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="680" activeTab="2" xr2:uid="{4ADEDBBA-C616-478B-B7B7-DF7FEDCE3438}"/>
   </bookViews>
   <sheets>
     <sheet name="Change History" sheetId="25" r:id="rId1"/>
@@ -23,7 +23,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="707">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="700">
   <si>
     <t>Title</t>
   </si>
@@ -1647,16 +1647,7 @@
     <t>Linked[Deliverables].ID</t>
   </si>
   <si>
-    <t>https://xyz.accenture.com/browse/PUAT1-1467</t>
-  </si>
-  <si>
-    <t>abc.d.xyz@mywizard.com</t>
-  </si>
-  <si>
     <t>2020-02-04T12:47:53Z</t>
-  </si>
-  <si>
-    <t>2020-02-04T12:49:55Z</t>
   </si>
   <si>
     <t>Epic1,Epic2;Story1,Story2;Feature2</t>
@@ -2091,18 +2082,12 @@
     <t>2021-08-02T06:12:57Z</t>
   </si>
   <si>
-    <t>BOM-118871</t>
-  </si>
-  <si>
     <t>Action_AutomationData_GenericUploader</t>
   </si>
   <si>
     <t>BOM</t>
   </si>
   <si>
-    <t>2021-08-02T08:22:23Z</t>
-  </si>
-  <si>
     <t>Plan</t>
   </si>
   <si>
@@ -2178,13 +2163,7 @@
     <t>Production</t>
   </si>
   <si>
-    <t>BOM-77679</t>
-  </si>
-  <si>
-    <t>2021-08-13T05:33:24Z</t>
-  </si>
-  <si>
-    <t>testuser01art@ds.dev.accenture.com</t>
+    <t>BOM-125496</t>
   </si>
 </sst>
 </file>
@@ -2194,7 +2173,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd\ hh:mm:ss"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3137,18 +3116,18 @@
       <selection activeCell="B22" sqref="B22:D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="7" width="10.77734375" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="2" width="59.44140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="4" width="16.21875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="4" width="11.88671875" collapsed="true"/>
-    <col min="5" max="5" style="4" width="8.77734375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="4" width="14.21875" collapsed="true"/>
-    <col min="7" max="16384" style="4" width="8.77734375" collapsed="true"/>
+    <col min="1" max="1" width="10.81640625" style="7" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="59.453125" style="2" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16.1796875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.90625" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.81640625" style="4" collapsed="1"/>
+    <col min="6" max="6" width="14.1796875" style="4" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="16384" width="8.81640625" style="4" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="13" t="s">
         <v>59</v>
       </c>
@@ -3162,374 +3141,374 @@
         <v>497</v>
       </c>
       <c r="E1" s="15" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="F1" s="15" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>598</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E6" s="19" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>607</v>
+        <v>604</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>609</v>
+        <v>606</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>605</v>
+        <v>602</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>611</v>
+        <v>608</v>
       </c>
       <c r="C10" s="18">
         <v>43992</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="76">
         <v>10</v>
       </c>
       <c r="B11" s="77" t="s">
-        <v>610</v>
+        <v>607</v>
       </c>
       <c r="C11" s="78">
         <v>44022</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E11" s="79"/>
       <c r="F11" s="6" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>628</v>
+        <v>625</v>
       </c>
       <c r="C12" s="18">
         <v>44022</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E12" s="6"/>
       <c r="F12" s="6" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>12</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>629</v>
+        <v>626</v>
       </c>
       <c r="C13" s="18">
         <v>44054</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E13" s="6"/>
       <c r="F13" s="6" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>627</v>
+        <v>624</v>
       </c>
       <c r="C14" s="18">
         <v>44054</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>14</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>630</v>
+        <v>627</v>
       </c>
       <c r="C15" s="18">
         <v>44054</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>15</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>631</v>
+        <v>628</v>
       </c>
       <c r="C16" s="18">
         <v>44054</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
       <c r="C17" s="18">
         <v>44120</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>642</v>
+        <v>639</v>
       </c>
       <c r="C18" s="18">
         <v>44125</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6" t="s">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>645</v>
+        <v>642</v>
       </c>
       <c r="C19" s="18">
         <v>44169</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="6" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" s="88">
         <v>19</v>
       </c>
       <c r="B20" s="89" t="s">
-        <v>653</v>
+        <v>650</v>
       </c>
       <c r="C20" s="90">
         <v>44263</v>
       </c>
       <c r="D20" s="91" t="s">
-        <v>646</v>
+        <v>643</v>
       </c>
       <c r="E20" s="91"/>
       <c r="F20" s="91"/>
     </row>
-    <row r="21" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="5">
         <v>20</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>661</v>
+        <v>658</v>
       </c>
       <c r="C21" s="18">
         <v>44363</v>
       </c>
       <c r="D21" s="60" t="s">
-        <v>662</v>
+        <v>659</v>
       </c>
       <c r="E21" s="6"/>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="7">
         <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>670</v>
+        <v>667</v>
       </c>
       <c r="C22" s="95">
         <v>44403</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>671</v>
+        <v>668</v>
       </c>
     </row>
   </sheetData>
@@ -3547,17 +3526,17 @@
       <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.21875" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="62.33203125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="27.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="1" width="15.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="50.33203125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="6.21875" collapsed="true"/>
-    <col min="6" max="16384" style="1" width="9.21875" collapsed="true"/>
+    <col min="1" max="1" width="62.36328125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="27.36328125" style="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15" style="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="50.36328125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="6.1796875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="16384" width="9.1796875" style="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A1" s="35" t="s">
         <v>45</v>
       </c>
@@ -3567,7 +3546,7 @@
         <v>46</v>
       </c>
       <c r="E1" s="37" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -3590,13 +3569,13 @@
       <c r="B3" s="39"/>
       <c r="C3" s="39"/>
       <c r="D3" s="40" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="E3" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="13" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>50</v>
       </c>
@@ -3607,7 +3586,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="25" x14ac:dyDescent="0.25">
       <c r="A5" s="45" t="s">
         <v>51</v>
       </c>
@@ -3620,14 +3599,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="25" x14ac:dyDescent="0.25">
       <c r="A6" s="47" t="s">
         <v>53</v>
       </c>
       <c r="B6" s="47"/>
       <c r="C6" s="47"/>
       <c r="D6" s="48" t="s">
-        <v>672</v>
+        <v>669</v>
       </c>
       <c r="E6" s="66" t="s">
         <v>49</v>
@@ -3640,26 +3619,26 @@
       <c r="B7" s="49"/>
       <c r="C7" s="49"/>
       <c r="D7" s="48" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="E7" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="25" x14ac:dyDescent="0.25">
       <c r="A8" s="67" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B8" s="49"/>
       <c r="C8" s="68"/>
       <c r="D8" s="69" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="E8" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="13.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="50" t="s">
         <v>55</v>
       </c>
@@ -3667,22 +3646,22 @@
         <v>58</v>
       </c>
       <c r="C9" s="70" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="D9" s="52" t="s">
         <v>1</v>
       </c>
       <c r="E9" s="53"/>
     </row>
-    <row r="10" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A10" s="54" t="s">
         <v>62</v>
       </c>
       <c r="B10" s="24" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="D10" s="34" t="s">
         <v>504</v>
@@ -3691,15 +3670,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A11" s="55" t="s">
         <v>64</v>
       </c>
       <c r="B11" s="24" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
       <c r="C11" s="33" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="D11" s="33" t="s">
         <v>505</v>
@@ -3708,7 +3687,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A12" s="56" t="s">
         <v>0</v>
       </c>
@@ -3716,7 +3695,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="33" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="D12" s="33" t="s">
         <v>506</v>
@@ -3725,7 +3704,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A13" s="55" t="s">
         <v>1</v>
       </c>
@@ -3733,7 +3712,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="33" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="D13" s="33" t="s">
         <v>507</v>
@@ -3742,7 +3721,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A14" s="55" t="s">
         <v>2</v>
       </c>
@@ -3750,7 +3729,7 @@
         <v>2</v>
       </c>
       <c r="C14" s="33" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="D14" s="33" t="s">
         <v>515</v>
@@ -3759,15 +3738,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A15" s="55" t="s">
         <v>3</v>
       </c>
       <c r="B15" s="82" t="s">
-        <v>644</v>
+        <v>641</v>
       </c>
       <c r="C15" s="33" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="D15" s="33" t="s">
         <v>508</v>
@@ -3776,32 +3755,32 @@
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="24" customFormat="1" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" s="24" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A16" s="55" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="B16" s="33" t="s">
-        <v>625</v>
+        <v>622</v>
       </c>
       <c r="C16" s="33" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="D16" s="33" t="s">
-        <v>626</v>
+        <v>623</v>
       </c>
       <c r="E16" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="26" x14ac:dyDescent="0.25">
       <c r="A17" s="55" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="B17" s="33" t="s">
         <v>498</v>
       </c>
       <c r="C17" s="33" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="D17" s="33" t="s">
         <v>509</v>
@@ -3810,32 +3789,32 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="24" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" s="24" customFormat="1" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="92" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="B18" s="82" t="s">
-        <v>655</v>
+        <v>652</v>
       </c>
       <c r="C18" s="84" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="D18" s="84" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="E18" s="85" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="24" customFormat="1" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" s="24" customFormat="1" ht="26" x14ac:dyDescent="0.25">
       <c r="A19" s="92" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="B19" s="82" t="s">
-        <v>657</v>
+        <v>654</v>
       </c>
       <c r="C19" s="84" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
       <c r="D19" s="84" t="s">
         <v>503</v>
@@ -3844,41 +3823,41 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A20" s="55" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="B20" s="33" t="s">
+        <v>612</v>
+      </c>
+      <c r="C20" s="33" t="s">
+        <v>583</v>
+      </c>
+      <c r="D20" s="80" t="s">
         <v>615</v>
-      </c>
-      <c r="C20" s="33" t="s">
-        <v>586</v>
-      </c>
-      <c r="D20" s="80" t="s">
-        <v>618</v>
       </c>
       <c r="E20" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A21" s="55" t="s">
+        <v>611</v>
+      </c>
+      <c r="B21" s="33" t="s">
+        <v>613</v>
+      </c>
+      <c r="C21" s="33" t="s">
+        <v>583</v>
+      </c>
+      <c r="D21" s="80" t="s">
         <v>614</v>
-      </c>
-      <c r="B21" s="33" t="s">
-        <v>616</v>
-      </c>
-      <c r="C21" s="33" t="s">
-        <v>586</v>
-      </c>
-      <c r="D21" s="80" t="s">
-        <v>617</v>
       </c>
       <c r="E21" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="69" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="65" x14ac:dyDescent="0.25">
       <c r="A22" s="55" t="s">
         <v>4</v>
       </c>
@@ -3886,135 +3865,135 @@
         <v>499</v>
       </c>
       <c r="C22" s="33" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="D22" s="33" t="s">
-        <v>643</v>
+        <v>640</v>
       </c>
       <c r="E22" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A23" s="55" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
       <c r="B23" s="33" t="s">
-        <v>547</v>
+        <v>544</v>
       </c>
       <c r="C23" s="33" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D23" s="33" t="s">
-        <v>666</v>
+        <v>663</v>
       </c>
       <c r="E23" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A24" s="55" t="s">
-        <v>548</v>
+        <v>545</v>
       </c>
       <c r="B24" s="33" t="s">
-        <v>549</v>
+        <v>546</v>
       </c>
       <c r="C24" s="33" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D24" s="33" t="s">
-        <v>667</v>
+        <v>664</v>
       </c>
       <c r="E24" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A25" s="55" t="s">
-        <v>550</v>
+        <v>547</v>
       </c>
       <c r="B25" s="33" t="s">
-        <v>551</v>
+        <v>548</v>
       </c>
       <c r="C25" s="33" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D25" s="33" t="s">
-        <v>669</v>
+        <v>666</v>
       </c>
       <c r="E25" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="52" x14ac:dyDescent="0.25">
       <c r="A26" s="55" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="B26" s="33" t="s">
-        <v>553</v>
+        <v>550</v>
       </c>
       <c r="C26" s="33" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D26" s="33" t="s">
-        <v>668</v>
+        <v>665</v>
       </c>
       <c r="E26" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A27" s="55" t="s">
-        <v>554</v>
+        <v>551</v>
       </c>
       <c r="B27" s="33" t="s">
-        <v>555</v>
+        <v>552</v>
       </c>
       <c r="C27" s="33" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D27" s="33" t="s">
-        <v>663</v>
+        <v>660</v>
       </c>
       <c r="E27" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="52" x14ac:dyDescent="0.25">
       <c r="A28" s="55" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="B28" s="33" t="s">
         <v>502</v>
       </c>
       <c r="C28" s="33" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D28" s="33" t="s">
-        <v>665</v>
+        <v>662</v>
       </c>
       <c r="E28" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="41.4" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A29" s="55" t="s">
         <v>6</v>
       </c>
       <c r="B29" s="33" t="s">
-        <v>557</v>
+        <v>554</v>
       </c>
       <c r="C29" s="33" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="D29" s="33" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="E29" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="52" x14ac:dyDescent="0.25">
       <c r="A30" s="55" t="s">
         <v>5</v>
       </c>
@@ -4022,7 +4001,7 @@
         <v>501</v>
       </c>
       <c r="C30" s="33" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="D30" s="33" t="s">
         <v>510</v>
@@ -4031,7 +4010,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="52" x14ac:dyDescent="0.25">
       <c r="A31" s="55" t="s">
         <v>8</v>
       </c>
@@ -4039,7 +4018,7 @@
         <v>500</v>
       </c>
       <c r="C31" s="33" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
       <c r="D31" s="33" t="s">
         <v>511</v>
@@ -4048,118 +4027,118 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="27.6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="26" x14ac:dyDescent="0.25">
       <c r="A32" s="55" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
       <c r="B32" s="33" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
       <c r="C32" s="33" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="D32" s="33" t="s">
         <v>512</v>
       </c>
       <c r="E32" s="23"/>
     </row>
-    <row r="33" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="39" x14ac:dyDescent="0.25">
       <c r="A33" s="55" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="B33" s="33" t="s">
-        <v>612</v>
+        <v>609</v>
       </c>
       <c r="C33" s="33" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
       <c r="D33" s="33" t="s">
-        <v>664</v>
+        <v>661</v>
       </c>
       <c r="E33" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A34" s="57" t="s">
-        <v>621</v>
+        <v>618</v>
       </c>
       <c r="B34" s="33" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
       <c r="C34" s="33" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
       <c r="D34" s="71" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
       <c r="E34" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="14.4" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A35" s="57" t="s">
-        <v>619</v>
+        <v>616</v>
       </c>
       <c r="B35" s="33" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
       <c r="C35" s="33" t="s">
+        <v>589</v>
+      </c>
+      <c r="D35" s="71" t="s">
         <v>592</v>
-      </c>
-      <c r="D35" s="71" t="s">
-        <v>595</v>
       </c>
       <c r="E35" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="52" x14ac:dyDescent="0.25">
       <c r="A36" s="55" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B36" s="33"/>
       <c r="C36" s="33" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D36" s="33" t="s">
-        <v>608</v>
+        <v>605</v>
       </c>
       <c r="E36" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="55.2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="52" x14ac:dyDescent="0.25">
       <c r="A37" s="57" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="B37" s="33"/>
       <c r="C37" s="72" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
       <c r="D37" s="33" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
       <c r="E37" s="66" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A38" s="87" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="B38" s="84"/>
       <c r="C38" s="86"/>
       <c r="D38" s="96" t="s">
-        <v>652</v>
+        <v>649</v>
       </c>
       <c r="E38" s="85" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A39" s="87" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="B39" s="84"/>
       <c r="C39" s="86"/>
@@ -4168,22 +4147,22 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A40" s="94" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="B40" s="84" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="C40" s="86" t="s">
-        <v>660</v>
+        <v>657</v>
       </c>
       <c r="D40" s="93"/>
       <c r="E40" s="85" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A41" s="94" t="s">
         <v>21</v>
       </c>
@@ -4191,14 +4170,14 @@
         <v>21</v>
       </c>
       <c r="C41" s="86" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
       <c r="D41" s="93"/>
       <c r="E41" s="85" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A42" s="59" t="s">
         <v>67</v>
       </c>
@@ -4211,14 +4190,14 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A43" s="26"/>
       <c r="B43" s="61"/>
       <c r="C43" s="61"/>
       <c r="D43" s="22"/>
       <c r="E43" s="22"/>
     </row>
-    <row r="44" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A44" s="62" t="s">
         <v>57</v>
       </c>
@@ -4227,7 +4206,7 @@
       <c r="D44" s="22"/>
       <c r="E44" s="22"/>
     </row>
-    <row r="45" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A45" s="47" t="s">
         <v>9</v>
       </c>
@@ -4240,7 +4219,7 @@
       </c>
       <c r="E45" s="22"/>
     </row>
-    <row r="46" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A46" s="47"/>
       <c r="B46" s="27" t="s">
         <v>17</v>
@@ -4251,7 +4230,7 @@
       </c>
       <c r="E46" s="22"/>
     </row>
-    <row r="47" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A47" s="47"/>
       <c r="B47" s="27" t="s">
         <v>20</v>
@@ -4262,7 +4241,7 @@
       </c>
       <c r="E47" s="22"/>
     </row>
-    <row r="48" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A48" s="47"/>
       <c r="B48" s="27" t="s">
         <v>23</v>
@@ -4273,7 +4252,7 @@
       </c>
       <c r="E48" s="22"/>
     </row>
-    <row r="49" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A49" s="47"/>
       <c r="B49" s="27" t="s">
         <v>25</v>
@@ -4284,7 +4263,7 @@
       </c>
       <c r="E49" s="22"/>
     </row>
-    <row r="50" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A50" s="47"/>
       <c r="B50" s="27" t="s">
         <v>29</v>
@@ -4295,7 +4274,7 @@
       </c>
       <c r="E50" s="22"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A51" s="47"/>
       <c r="B51" s="27" t="s">
         <v>30</v>
@@ -4305,7 +4284,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A52" s="47"/>
       <c r="B52" s="27" t="s">
         <v>31</v>
@@ -4315,7 +4294,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A53" s="47"/>
       <c r="B53" s="27" t="s">
         <v>32</v>
@@ -4325,7 +4304,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A54" s="47"/>
       <c r="B54" s="27" t="s">
         <v>65</v>
@@ -4335,7 +4314,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A55" s="47"/>
       <c r="B55" s="27" t="s">
         <v>66</v>
@@ -4345,7 +4324,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A56" s="47"/>
       <c r="B56" s="27" t="s">
         <v>513</v>
@@ -4353,7 +4332,7 @@
       <c r="C56" s="27"/>
       <c r="D56" s="48"/>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A57" s="47"/>
       <c r="B57" s="27" t="s">
         <v>10</v>
@@ -4361,7 +4340,7 @@
       <c r="C57" s="27"/>
       <c r="D57" s="48"/>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A58" s="47" t="s">
         <v>5</v>
       </c>
@@ -4373,7 +4352,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A59" s="47"/>
       <c r="B59" s="28" t="s">
         <v>15</v>
@@ -4383,7 +4362,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A60" s="47"/>
       <c r="B60" s="28" t="s">
         <v>18</v>
@@ -4393,7 +4372,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A61" s="47"/>
       <c r="B61" s="28" t="s">
         <v>21</v>
@@ -4403,7 +4382,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A62" s="47"/>
       <c r="B62" s="28" t="s">
         <v>24</v>
@@ -4413,7 +4392,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A63" s="47"/>
       <c r="B63" s="29" t="s">
         <v>26</v>
@@ -4423,12 +4402,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" ht="13" x14ac:dyDescent="0.25">
       <c r="A64" s="47" t="s">
         <v>67</v>
       </c>
       <c r="B64" s="30" t="s">
-        <v>658</v>
+        <v>655</v>
       </c>
       <c r="C64" s="30"/>
       <c r="D64" s="48" t="s">
@@ -7003,7 +6982,7 @@
       <c r="C354" s="63"/>
       <c r="D354" s="48"/>
     </row>
-    <row r="355" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="355" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A355" s="31" t="s">
         <v>8</v>
       </c>
@@ -7013,7 +6992,7 @@
       <c r="C355" s="32"/>
       <c r="D355" s="48"/>
     </row>
-    <row r="356" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="356" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A356" s="31"/>
       <c r="B356" s="32" t="s">
         <v>34</v>
@@ -7021,7 +7000,7 @@
       <c r="C356" s="32"/>
       <c r="D356" s="48"/>
     </row>
-    <row r="357" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="357" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A357" s="47"/>
       <c r="B357" s="32" t="s">
         <v>14</v>
@@ -7029,7 +7008,7 @@
       <c r="C357" s="32"/>
       <c r="D357" s="48"/>
     </row>
-    <row r="358" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="358" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A358" s="47"/>
       <c r="B358" s="32" t="s">
         <v>35</v>
@@ -7037,7 +7016,7 @@
       <c r="C358" s="32"/>
       <c r="D358" s="48"/>
     </row>
-    <row r="359" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="359" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A359" s="47"/>
       <c r="B359" s="32" t="s">
         <v>12</v>
@@ -7045,7 +7024,7 @@
       <c r="C359" s="32"/>
       <c r="D359" s="48"/>
     </row>
-    <row r="360" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="360" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A360" s="47"/>
       <c r="B360" s="32" t="s">
         <v>36</v>
@@ -7053,7 +7032,7 @@
       <c r="C360" s="32"/>
       <c r="D360" s="48"/>
     </row>
-    <row r="361" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="361" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A361" s="47"/>
       <c r="B361" s="32" t="s">
         <v>37</v>
@@ -7061,7 +7040,7 @@
       <c r="C361" s="32"/>
       <c r="D361" s="48"/>
     </row>
-    <row r="362" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="362" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A362" s="47"/>
       <c r="B362" s="32" t="s">
         <v>33</v>
@@ -7069,7 +7048,7 @@
       <c r="C362" s="32"/>
       <c r="D362" s="48"/>
     </row>
-    <row r="363" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="363" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A363" s="47"/>
       <c r="B363" s="32" t="s">
         <v>16</v>
@@ -7077,7 +7056,7 @@
       <c r="C363" s="32"/>
       <c r="D363" s="48"/>
     </row>
-    <row r="364" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="364" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A364" s="47"/>
       <c r="B364" s="32" t="s">
         <v>19</v>
@@ -7085,7 +7064,7 @@
       <c r="C364" s="32"/>
       <c r="D364" s="48"/>
     </row>
-    <row r="365" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="365" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A365" s="47"/>
       <c r="B365" s="32" t="s">
         <v>22</v>
@@ -7093,7 +7072,7 @@
       <c r="C365" s="32"/>
       <c r="D365" s="48"/>
     </row>
-    <row r="366" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="366" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A366" s="47"/>
       <c r="B366" s="32" t="s">
         <v>483</v>
@@ -7101,7 +7080,7 @@
       <c r="C366" s="32"/>
       <c r="D366" s="48"/>
     </row>
-    <row r="367" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="367" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A367" s="47"/>
       <c r="B367" s="32" t="s">
         <v>28</v>
@@ -7109,7 +7088,7 @@
       <c r="C367" s="32"/>
       <c r="D367" s="48"/>
     </row>
-    <row r="368" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="368" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A368" s="47"/>
       <c r="B368" s="32" t="s">
         <v>484</v>
@@ -7117,7 +7096,7 @@
       <c r="C368" s="32"/>
       <c r="D368" s="48"/>
     </row>
-    <row r="369" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="369" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A369" s="47"/>
       <c r="B369" s="32" t="s">
         <v>485</v>
@@ -7125,7 +7104,7 @@
       <c r="C369" s="32"/>
       <c r="D369" s="48"/>
     </row>
-    <row r="370" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="370" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A370" s="47"/>
       <c r="B370" s="32" t="s">
         <v>486</v>
@@ -7133,7 +7112,7 @@
       <c r="C370" s="32"/>
       <c r="D370" s="48"/>
     </row>
-    <row r="371" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="371" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A371" s="47"/>
       <c r="B371" s="32" t="s">
         <v>487</v>
@@ -7141,7 +7120,7 @@
       <c r="C371" s="32"/>
       <c r="D371" s="48"/>
     </row>
-    <row r="372" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="372" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A372" s="47"/>
       <c r="B372" s="32" t="s">
         <v>488</v>
@@ -7149,7 +7128,7 @@
       <c r="C372" s="32"/>
       <c r="D372" s="48"/>
     </row>
-    <row r="373" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="373" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A373" s="47"/>
       <c r="B373" s="32" t="s">
         <v>489</v>
@@ -7157,7 +7136,7 @@
       <c r="C373" s="32"/>
       <c r="D373" s="48"/>
     </row>
-    <row r="374" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="374" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A374" s="47"/>
       <c r="B374" s="32" t="s">
         <v>490</v>
@@ -7165,7 +7144,7 @@
       <c r="C374" s="32"/>
       <c r="D374" s="48"/>
     </row>
-    <row r="375" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="375" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A375" s="47"/>
       <c r="B375" s="32" t="s">
         <v>491</v>
@@ -7173,7 +7152,7 @@
       <c r="C375" s="32"/>
       <c r="D375" s="48"/>
     </row>
-    <row r="376" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="376" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A376" s="47"/>
       <c r="B376" s="32" t="s">
         <v>492</v>
@@ -7181,7 +7160,7 @@
       <c r="C376" s="32"/>
       <c r="D376" s="48"/>
     </row>
-    <row r="377" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="377" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A377" s="47"/>
       <c r="B377" s="32" t="s">
         <v>493</v>
@@ -7189,7 +7168,7 @@
       <c r="C377" s="32"/>
       <c r="D377" s="48"/>
     </row>
-    <row r="378" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="378" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A378" s="47"/>
       <c r="B378" s="32" t="s">
         <v>494</v>
@@ -7197,7 +7176,7 @@
       <c r="C378" s="32"/>
       <c r="D378" s="48"/>
     </row>
-    <row r="379" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="379" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A379" s="47"/>
       <c r="B379" s="32" t="s">
         <v>495</v>
@@ -7205,7 +7184,7 @@
       <c r="C379" s="32"/>
       <c r="D379" s="48"/>
     </row>
-    <row r="380" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A380" s="48" t="s">
         <v>7</v>
       </c>
@@ -7215,7 +7194,7 @@
       <c r="C380" s="73"/>
       <c r="D380" s="22"/>
     </row>
-    <row r="381" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A381" s="22"/>
       <c r="B381" s="32" t="s">
         <v>496</v>
@@ -7223,7 +7202,7 @@
       <c r="C381" s="73"/>
       <c r="D381" s="22"/>
     </row>
-    <row r="382" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A382" s="22"/>
       <c r="B382" s="32" t="s">
         <v>27</v>
@@ -7231,23 +7210,23 @@
       <c r="C382" s="73"/>
       <c r="D382" s="22"/>
     </row>
-    <row r="383" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A383" s="58" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
       <c r="B383" s="22"/>
       <c r="C383" s="22"/>
       <c r="D383" s="22"/>
     </row>
-    <row r="384" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A384" s="22"/>
       <c r="B384" s="64" t="s">
-        <v>561</v>
+        <v>558</v>
       </c>
       <c r="C384" s="74"/>
       <c r="D384" s="22"/>
     </row>
-    <row r="385" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A385" s="22"/>
       <c r="B385" s="64" t="s">
         <v>34</v>
@@ -7255,7 +7234,7 @@
       <c r="C385" s="74"/>
       <c r="D385" s="22"/>
     </row>
-    <row r="386" spans="1:4" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:4" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A386" s="22"/>
       <c r="B386" s="64" t="s">
         <v>14</v>
@@ -7263,133 +7242,133 @@
       <c r="C386" s="74"/>
       <c r="D386" s="22"/>
     </row>
-    <row r="387" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="387" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="B387" s="64" t="s">
         <v>35</v>
       </c>
       <c r="C387" s="74"/>
     </row>
-    <row r="388" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="388" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="B388" s="64" t="s">
         <v>12</v>
       </c>
       <c r="C388" s="74"/>
     </row>
-    <row r="389" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="389" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="B389" s="64" t="s">
         <v>36</v>
       </c>
       <c r="C389" s="74"/>
     </row>
-    <row r="390" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="390" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="B390" s="64" t="s">
         <v>37</v>
       </c>
       <c r="C390" s="74"/>
     </row>
-    <row r="391" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="391" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="B391" s="64" t="s">
         <v>33</v>
       </c>
       <c r="C391" s="74"/>
     </row>
-    <row r="392" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="392" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="B392" s="65" t="s">
         <v>16</v>
       </c>
       <c r="C392" s="75"/>
     </row>
-    <row r="393" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="393" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="B393" s="65" t="s">
         <v>19</v>
       </c>
       <c r="C393" s="75"/>
     </row>
-    <row r="394" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="394" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="B394" s="65" t="s">
         <v>22</v>
       </c>
       <c r="C394" s="75"/>
     </row>
-    <row r="395" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="395" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="B395" s="65" t="s">
         <v>483</v>
       </c>
       <c r="C395" s="75"/>
     </row>
-    <row r="396" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="396" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="B396" s="65" t="s">
         <v>28</v>
       </c>
       <c r="C396" s="75"/>
     </row>
-    <row r="397" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="397" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="B397" s="65" t="s">
         <v>484</v>
       </c>
       <c r="C397" s="75"/>
     </row>
-    <row r="398" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="398" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="B398" s="65" t="s">
         <v>485</v>
       </c>
       <c r="C398" s="75"/>
     </row>
-    <row r="399" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="399" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="B399" s="65" t="s">
         <v>486</v>
       </c>
       <c r="C399" s="75"/>
     </row>
-    <row r="400" spans="1:4" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="400" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="B400" s="65" t="s">
         <v>487</v>
       </c>
       <c r="C400" s="75"/>
     </row>
-    <row r="401" spans="2:3" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="401" spans="2:3" ht="13" x14ac:dyDescent="0.25">
       <c r="B401" s="65" t="s">
         <v>488</v>
       </c>
       <c r="C401" s="75"/>
     </row>
-    <row r="402" spans="2:3" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="402" spans="2:3" ht="13" x14ac:dyDescent="0.25">
       <c r="B402" s="65" t="s">
         <v>489</v>
       </c>
       <c r="C402" s="75"/>
     </row>
-    <row r="403" spans="2:3" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="403" spans="2:3" ht="13" x14ac:dyDescent="0.25">
       <c r="B403" s="65" t="s">
         <v>490</v>
       </c>
       <c r="C403" s="75"/>
     </row>
-    <row r="404" spans="2:3" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="404" spans="2:3" ht="13" x14ac:dyDescent="0.25">
       <c r="B404" s="65" t="s">
         <v>491</v>
       </c>
       <c r="C404" s="75"/>
     </row>
-    <row r="405" spans="2:3" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="405" spans="2:3" ht="13" x14ac:dyDescent="0.25">
       <c r="B405" s="65" t="s">
         <v>492</v>
       </c>
       <c r="C405" s="75"/>
     </row>
-    <row r="406" spans="2:3" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="406" spans="2:3" ht="13" x14ac:dyDescent="0.25">
       <c r="B406" s="65" t="s">
         <v>493</v>
       </c>
       <c r="C406" s="75"/>
     </row>
-    <row r="407" spans="2:3" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="407" spans="2:3" ht="13" x14ac:dyDescent="0.25">
       <c r="B407" s="65" t="s">
         <v>494</v>
       </c>
       <c r="C407" s="75"/>
     </row>
-    <row r="408" spans="2:3" ht="13.8" x14ac:dyDescent="0.25">
+    <row r="408" spans="2:3" ht="13" x14ac:dyDescent="0.25">
       <c r="B408" s="65" t="s">
         <v>495</v>
       </c>
@@ -7409,65 +7388,65 @@
   <dimension ref="A1:BM2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.88671875" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="41.21875" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="23.21875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" style="22" width="23.21875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="22.77734375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="22" width="22.77734375" collapsed="true"/>
-    <col min="8" max="11" bestFit="true" customWidth="true" width="22.77734375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.21875" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="15.5546875" collapsed="true"/>
-    <col min="14" max="16" bestFit="true" customWidth="true" width="19.21875" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="19.5546875" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="17.21875" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="15.21875" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="5.21875" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="7.44140625" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" width="18.44140625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="11.77734375" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="19.5546875" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="19.77734375" collapsed="true"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" width="20.21875" collapsed="true"/>
-    <col min="28" max="31" customWidth="true" style="22" width="20.21875" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" width="10.6640625" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="19.21875" collapsed="true"/>
-    <col min="34" max="34" bestFit="true" customWidth="true" width="22.88671875" collapsed="true"/>
-    <col min="35" max="35" bestFit="true" customWidth="true" width="17.33203125" collapsed="true"/>
-    <col min="36" max="36" bestFit="true" customWidth="true" width="26.109375" collapsed="true"/>
-    <col min="37" max="37" bestFit="true" customWidth="true" width="19.6640625" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="28.33203125" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="14.6640625" collapsed="true"/>
-    <col min="40" max="40" bestFit="true" customWidth="true" width="53.6640625" collapsed="true"/>
-    <col min="41" max="41" bestFit="true" customWidth="true" width="53.21875" collapsed="true"/>
-    <col min="42" max="42" bestFit="true" customWidth="true" width="29.88671875" collapsed="true"/>
-    <col min="43" max="43" bestFit="true" customWidth="true" width="21.21875" collapsed="true"/>
-    <col min="44" max="44" bestFit="true" customWidth="true" width="30.0" collapsed="true"/>
-    <col min="45" max="45" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="46" max="46" bestFit="true" customWidth="true" width="29.88671875" collapsed="true"/>
-    <col min="47" max="47" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="48" max="48" bestFit="true" customWidth="true" width="22.88671875" collapsed="true"/>
-    <col min="49" max="49" bestFit="true" customWidth="true" width="16.21875" collapsed="true"/>
-    <col min="50" max="50" bestFit="true" customWidth="true" style="22" width="17.88671875" collapsed="true"/>
-    <col min="51" max="51" bestFit="true" customWidth="true" style="22" width="26.6640625" collapsed="true"/>
-    <col min="52" max="52" bestFit="true" customWidth="true" width="24.88671875" collapsed="true"/>
-    <col min="53" max="53" bestFit="true" customWidth="true" width="20.21875" collapsed="true"/>
-    <col min="54" max="54" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
-    <col min="55" max="55" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="56" max="56" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
-    <col min="57" max="57" bestFit="true" customWidth="true" width="23.109375" collapsed="true"/>
-    <col min="63" max="63" bestFit="true" customWidth="true" width="24.6640625" collapsed="true"/>
-    <col min="64" max="64" bestFit="true" customWidth="true" width="19.5546875" collapsed="true"/>
-    <col min="65" max="65" bestFit="true" customWidth="true" width="29.0" collapsed="true"/>
+    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="41.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="4" width="23.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="23.1796875" style="22" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="22.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="22.81640625" style="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="11" width="22.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="19.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="15.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="16" width="19.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="19.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="17.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="5.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="14" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="7.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="18.453125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="11.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="19.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="19.81640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="27" max="27" width="20.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="28" max="31" width="20.1796875" style="22" customWidth="1" collapsed="1"/>
+    <col min="32" max="32" width="10.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="33" max="33" width="19.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="22.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="35" max="35" width="17.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="36" max="36" width="26.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="37" max="37" width="19.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="38" max="38" width="28.36328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="39" max="39" width="14.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="40" max="40" width="53.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="41" max="41" width="53.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="42" max="42" width="29.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="43" max="43" width="21.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="44" max="44" width="30" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="45" max="45" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="46" max="46" width="29.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="47" max="47" width="18" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="48" max="48" width="22.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="49" max="49" width="16.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="50" max="50" width="17.90625" style="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="51" max="51" width="26.6328125" style="22" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="52" max="52" width="24.90625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="53" max="53" width="20.1796875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="54" max="54" width="29" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="55" max="55" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="56" max="56" width="27" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="57" max="57" width="23.08984375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="63" max="63" width="24.6328125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="64" max="64" width="19.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="65" max="65" width="29" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:65" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:65" x14ac:dyDescent="0.35">
       <c r="A1" s="9" t="s">
         <v>62</v>
       </c>
@@ -7481,46 +7460,46 @@
         <v>1</v>
       </c>
       <c r="E1" s="9" t="s">
-        <v>673</v>
+        <v>670</v>
       </c>
       <c r="F1" s="20" t="s">
         <v>3</v>
       </c>
       <c r="G1" s="10" t="s">
-        <v>624</v>
+        <v>621</v>
       </c>
       <c r="H1" s="20" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="I1" s="87" t="s">
-        <v>654</v>
+        <v>651</v>
       </c>
       <c r="J1" s="87" t="s">
-        <v>656</v>
+        <v>653</v>
       </c>
       <c r="K1" s="20" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="L1" s="20" t="s">
+        <v>542</v>
+      </c>
+      <c r="M1" s="20" t="s">
+        <v>543</v>
+      </c>
+      <c r="N1" s="20" t="s">
+        <v>547</v>
+      </c>
+      <c r="O1" s="20" t="s">
+        <v>551</v>
+      </c>
+      <c r="P1" s="20" t="s">
         <v>545</v>
       </c>
-      <c r="M1" s="20" t="s">
-        <v>546</v>
-      </c>
-      <c r="N1" s="20" t="s">
-        <v>550</v>
-      </c>
-      <c r="O1" s="20" t="s">
-        <v>554</v>
-      </c>
-      <c r="P1" s="20" t="s">
-        <v>548</v>
-      </c>
       <c r="Q1" s="20" t="s">
-        <v>552</v>
+        <v>549</v>
       </c>
       <c r="R1" s="20" t="s">
-        <v>556</v>
+        <v>553</v>
       </c>
       <c r="S1" s="21" t="s">
         <v>4</v>
@@ -7535,28 +7514,28 @@
         <v>8</v>
       </c>
       <c r="W1" s="20" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="X1" s="17" t="s">
-        <v>620</v>
+        <v>617</v>
       </c>
       <c r="Y1" s="17" t="s">
-        <v>632</v>
+        <v>629</v>
       </c>
       <c r="Z1" s="20" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="AA1" s="20" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="AB1" s="20" t="s">
-        <v>650</v>
+        <v>647</v>
       </c>
       <c r="AC1" s="20" t="s">
-        <v>651</v>
+        <v>648</v>
       </c>
       <c r="AD1" s="20" t="s">
-        <v>659</v>
+        <v>656</v>
       </c>
       <c r="AE1" s="20" t="s">
         <v>21</v>
@@ -7610,16 +7589,16 @@
         <v>521</v>
       </c>
       <c r="AV1" s="8" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="AW1" s="8" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="AX1" s="8" t="s">
-        <v>622</v>
+        <v>619</v>
       </c>
       <c r="AY1" s="8" t="s">
-        <v>623</v>
+        <v>620</v>
       </c>
       <c r="AZ1" s="8" t="s">
         <v>533</v>
@@ -7628,116 +7607,94 @@
         <v>522</v>
       </c>
       <c r="BB1" s="8" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="BC1" s="8" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="BD1" s="8" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="BE1" s="8" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="BF1" s="8" t="s">
+        <v>630</v>
+      </c>
+      <c r="BG1" s="8" t="s">
+        <v>631</v>
+      </c>
+      <c r="BH1" s="8" t="s">
+        <v>632</v>
+      </c>
+      <c r="BI1" s="8" t="s">
         <v>633</v>
       </c>
-      <c r="BG1" s="8" t="s">
+      <c r="BJ1" s="81" t="s">
         <v>634</v>
       </c>
-      <c r="BH1" s="8" t="s">
+      <c r="BK1" s="81" t="s">
         <v>635</v>
       </c>
-      <c r="BI1" s="8" t="s">
+      <c r="BL1" s="83" t="s">
+        <v>645</v>
+      </c>
+      <c r="BM1" s="83" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="2" spans="1:65" x14ac:dyDescent="0.35">
+      <c r="A2" s="12" t="s">
+        <v>699</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="12" t="s">
+        <v>672</v>
+      </c>
+      <c r="D2" s="12" t="s">
         <v>636</v>
       </c>
-      <c r="BJ1" s="81" t="s">
-        <v>637</v>
-      </c>
-      <c r="BK1" s="81" t="s">
-        <v>638</v>
-      </c>
-      <c r="BL1" s="83" t="s">
-        <v>648</v>
-      </c>
-      <c r="BM1" s="83" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="2" spans="1:65" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
-        <v>704</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>534</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>676</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>639</v>
-      </c>
       <c r="E2" s="12" t="s">
-        <v>677</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>706</v>
-      </c>
+        <v>673</v>
+      </c>
+      <c r="F2" s="16"/>
       <c r="G2" s="12"/>
       <c r="H2" s="16"/>
-      <c r="I2" s="16" t="s">
-        <v>535</v>
-      </c>
-      <c r="J2" s="16" t="s">
-        <v>535</v>
-      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
       <c r="K2" s="11" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="L2" s="11" t="s">
-        <v>674</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>705</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>536</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>537</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>537</v>
-      </c>
-      <c r="Q2" s="11" t="s">
-        <v>536</v>
-      </c>
-      <c r="R2" s="11" t="s">
-        <v>536</v>
-      </c>
+        <v>671</v>
+      </c>
+      <c r="M2" s="11"/>
+      <c r="N2" s="11"/>
+      <c r="O2" s="11"/>
+      <c r="P2" s="11"/>
+      <c r="Q2" s="11"/>
+      <c r="R2" s="11"/>
       <c r="S2" s="11"/>
       <c r="T2" s="12"/>
       <c r="U2" s="12"/>
       <c r="V2" s="12"/>
-      <c r="W2" s="11" t="s">
-        <v>536</v>
-      </c>
+      <c r="W2" s="11"/>
       <c r="Y2" s="12"/>
       <c r="Z2" s="12"/>
       <c r="AA2" s="12"/>
       <c r="AB2" s="12"/>
       <c r="AC2" s="12"/>
       <c r="AD2" s="12" t="s">
-        <v>679</v>
+        <v>674</v>
       </c>
       <c r="AE2" s="12" t="s">
-        <v>680</v>
+        <v>675</v>
       </c>
       <c r="AF2" s="12" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="AG2" s="12" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="AI2" s="12"/>
       <c r="AJ2" s="12"/>
@@ -7830,23 +7787,23 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="1" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E1" t="s">
-        <v>681</v>
+        <v>676</v>
       </c>
       <c r="F1" t="s">
         <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>682</v>
+        <v>677</v>
       </c>
       <c r="H1" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="I1" t="s">
-        <v>683</v>
+        <v>678</v>
       </c>
       <c r="J1" t="s">
         <v>10</v>
@@ -7855,38 +7812,38 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E2" t="s">
-        <v>684</v>
+        <v>679</v>
       </c>
       <c r="F2" t="s">
         <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>685</v>
+        <v>680</v>
       </c>
       <c r="H2" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="I2" t="s">
-        <v>686</v>
+        <v>681</v>
       </c>
       <c r="J2" t="s">
         <v>15</v>
       </c>
       <c r="K2" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="3" spans="5:11" x14ac:dyDescent="0.3">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="3" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E3" t="s">
-        <v>688</v>
+        <v>683</v>
       </c>
       <c r="F3" t="s">
         <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>689</v>
+        <v>684</v>
       </c>
       <c r="J3" t="s">
         <v>18</v>
@@ -7895,32 +7852,32 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E4" t="s">
-        <v>690</v>
+        <v>685</v>
       </c>
       <c r="F4" t="s">
         <v>35</v>
       </c>
       <c r="G4" t="s">
-        <v>691</v>
+        <v>686</v>
       </c>
       <c r="J4" t="s">
         <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>692</v>
-      </c>
-    </row>
-    <row r="5" spans="5:11" x14ac:dyDescent="0.3">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="5" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E5" t="s">
-        <v>693</v>
+        <v>688</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
       </c>
       <c r="G5" t="s">
-        <v>694</v>
+        <v>689</v>
       </c>
       <c r="J5" t="s">
         <v>24</v>
@@ -7929,9 +7886,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E6" t="s">
-        <v>695</v>
+        <v>690</v>
       </c>
       <c r="F6" t="s">
         <v>36</v>
@@ -7943,53 +7900,53 @@
         <v>26</v>
       </c>
       <c r="K6" t="s">
-        <v>696</v>
-      </c>
-    </row>
-    <row r="7" spans="5:11" x14ac:dyDescent="0.3">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="7" spans="5:11" x14ac:dyDescent="0.35">
       <c r="E7" t="s">
-        <v>697</v>
+        <v>692</v>
       </c>
       <c r="F7" t="s">
         <v>37</v>
       </c>
       <c r="K7" t="s">
-        <v>698</v>
-      </c>
-    </row>
-    <row r="8" spans="5:11" x14ac:dyDescent="0.3">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="8" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F8" t="s">
         <v>33</v>
       </c>
       <c r="K8" t="s">
-        <v>699</v>
-      </c>
-    </row>
-    <row r="9" spans="5:11" x14ac:dyDescent="0.3">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="9" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F9" t="s">
         <v>16</v>
       </c>
       <c r="K9" t="s">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="10" spans="5:11" x14ac:dyDescent="0.3">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="10" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F10" t="s">
         <v>19</v>
       </c>
       <c r="K10" t="s">
-        <v>701</v>
-      </c>
-    </row>
-    <row r="11" spans="5:11" x14ac:dyDescent="0.3">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="11" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F11" t="s">
         <v>22</v>
       </c>
       <c r="K11" t="s">
-        <v>702</v>
-      </c>
-    </row>
-    <row r="12" spans="5:11" x14ac:dyDescent="0.3">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="12" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F12" t="s">
         <v>483</v>
       </c>
@@ -7997,70 +7954,70 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="13" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F13" t="s">
         <v>28</v>
       </c>
       <c r="K13" t="s">
-        <v>703</v>
-      </c>
-    </row>
-    <row r="14" spans="5:11" x14ac:dyDescent="0.3">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="14" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F14" t="s">
         <v>484</v>
       </c>
     </row>
-    <row r="15" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F15" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="16" spans="5:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="5:11" x14ac:dyDescent="0.35">
       <c r="F16" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F17" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F18" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F19" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F20" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F21" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F22" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F23" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="24" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F24" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="25" spans="6:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="6:6" x14ac:dyDescent="0.35">
       <c r="F25" t="s">
         <v>495</v>
       </c>
@@ -8072,6 +8029,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F589723C5CF9BF4888831BB2DC69A718" ma:contentTypeVersion="6" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e7d91ee2624ae14a4be9994568eb03d9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bc0735e1-1781-4e64-a3a6-cf1bacd21285" xmlns:ns3="acee2d6b-dd79-4fb3-8fb4-89e5568edfef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="bf92cc8814d37b02d77c323fc2a11963" ns2:_="" ns3:_="">
     <xsd:import namespace="bc0735e1-1781-4e64-a3a6-cf1bacd21285"/>
@@ -8250,36 +8222,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{090AF72E-503D-4D63-A8FB-B98DEABA3FFD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F359188-8654-4AC8-AEDD-04D6FE3DA0A5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bc0735e1-1781-4e64-a3a6-cf1bacd21285"/>
-    <ds:schemaRef ds:uri="acee2d6b-dd79-4fb3-8fb4-89e5568edfef"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8302,9 +8248,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1F359188-8654-4AC8-AEDD-04D6FE3DA0A5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{090AF72E-503D-4D63-A8FB-B98DEABA3FFD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bc0735e1-1781-4e64-a3a6-cf1bacd21285"/>
+    <ds:schemaRef ds:uri="acee2d6b-dd79-4fb3-8fb4-89e5568edfef"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>